<commit_message>
update occupation classification code
</commit_message>
<xml_diff>
--- a/S2022/comparison_between_debt_holders/avg_debt_occupation/FinishedSpreadsheets/OccupationsAllStates.xlsx
+++ b/S2022/comparison_between_debt_holders/avg_debt_occupation/FinishedSpreadsheets/OccupationsAllStates.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>occupation</t>
   </si>
@@ -25,232 +25,235 @@
     <t># of people</t>
   </si>
   <si>
+    <t>% of total people</t>
+  </si>
+  <si>
     <t>average debt per person</t>
   </si>
   <si>
+    <t>merchant</t>
+  </si>
+  <si>
+    <t>treasurer</t>
+  </si>
+  <si>
+    <t>esq</t>
+  </si>
+  <si>
+    <t>broker</t>
+  </si>
+  <si>
+    <t>farmer</t>
+  </si>
+  <si>
+    <t>gentleman</t>
+  </si>
+  <si>
+    <t>widow</t>
+  </si>
+  <si>
+    <t>doctor</t>
+  </si>
+  <si>
+    <t>attorney</t>
+  </si>
+  <si>
+    <t>excuetor</t>
+  </si>
+  <si>
+    <t>trader</t>
+  </si>
+  <si>
+    <t>mariner</t>
+  </si>
+  <si>
+    <t>planter</t>
+  </si>
+  <si>
     <t>adminastrator</t>
   </si>
   <si>
+    <t>printer</t>
+  </si>
+  <si>
+    <t>post master</t>
+  </si>
+  <si>
+    <t>guardian</t>
+  </si>
+  <si>
+    <t>blockmaker</t>
+  </si>
+  <si>
+    <t>druggist</t>
+  </si>
+  <si>
+    <t>clerk</t>
+  </si>
+  <si>
+    <t>shoemaker</t>
+  </si>
+  <si>
+    <t>taylor</t>
+  </si>
+  <si>
+    <t>sadler</t>
+  </si>
+  <si>
+    <t>blacksmith</t>
+  </si>
+  <si>
+    <t>spinster</t>
+  </si>
+  <si>
+    <t>hatter</t>
+  </si>
+  <si>
+    <t>inn keeper</t>
+  </si>
+  <si>
+    <t>furrier</t>
+  </si>
+  <si>
+    <t>sheriff</t>
+  </si>
+  <si>
+    <t>trustee</t>
+  </si>
+  <si>
+    <t>assignee</t>
+  </si>
+  <si>
+    <t>baker</t>
+  </si>
+  <si>
+    <t>school master</t>
+  </si>
+  <si>
+    <t>tanner</t>
+  </si>
+  <si>
+    <t>reverend</t>
+  </si>
+  <si>
+    <t>judges</t>
+  </si>
+  <si>
+    <t>ship wright</t>
+  </si>
+  <si>
+    <t>estate</t>
+  </si>
+  <si>
+    <t>silversmith</t>
+  </si>
+  <si>
+    <t>cooper</t>
+  </si>
+  <si>
+    <t>mason</t>
+  </si>
+  <si>
+    <t>school committee</t>
+  </si>
+  <si>
+    <t>goldsmith</t>
+  </si>
+  <si>
+    <t>glazier</t>
+  </si>
+  <si>
+    <t>committee</t>
+  </si>
+  <si>
+    <t>individual</t>
+  </si>
+  <si>
+    <t>shopkeeper</t>
+  </si>
+  <si>
+    <t>carpenter</t>
+  </si>
+  <si>
+    <t>book binder</t>
+  </si>
+  <si>
+    <t>post rider</t>
+  </si>
+  <si>
+    <t>leather dresser</t>
+  </si>
+  <si>
+    <t>auctioneer</t>
+  </si>
+  <si>
+    <t>distiller</t>
+  </si>
+  <si>
+    <t>property</t>
+  </si>
+  <si>
+    <t>proprietors</t>
+  </si>
+  <si>
+    <t>cordwainder</t>
+  </si>
+  <si>
+    <t>housewright</t>
+  </si>
+  <si>
+    <t>butcher</t>
+  </si>
+  <si>
+    <t>molster</t>
+  </si>
+  <si>
+    <t>frederick company</t>
+  </si>
+  <si>
+    <t>conveyancer</t>
+  </si>
+  <si>
+    <t>cashier</t>
+  </si>
+  <si>
+    <t>soldier</t>
+  </si>
+  <si>
+    <t>cabinet maker</t>
+  </si>
+  <si>
+    <t>labourer</t>
+  </si>
+  <si>
+    <t>wife</t>
+  </si>
+  <si>
+    <t>comtroller</t>
+  </si>
+  <si>
+    <t>clothier</t>
+  </si>
+  <si>
+    <t>painter</t>
+  </si>
+  <si>
+    <t>chaise maker</t>
+  </si>
+  <si>
+    <t>weaver</t>
+  </si>
+  <si>
+    <t>bricklayer</t>
+  </si>
+  <si>
+    <t>miller</t>
+  </si>
+  <si>
+    <t>deacon</t>
+  </si>
+  <si>
     <t>apothecary</t>
-  </si>
-  <si>
-    <t>assignee</t>
-  </si>
-  <si>
-    <t>attorney</t>
-  </si>
-  <si>
-    <t>auctioneer</t>
-  </si>
-  <si>
-    <t>baker</t>
-  </si>
-  <si>
-    <t>blacksmith</t>
-  </si>
-  <si>
-    <t>blockmaker</t>
-  </si>
-  <si>
-    <t>book binder</t>
-  </si>
-  <si>
-    <t>bricklayer</t>
-  </si>
-  <si>
-    <t>broker</t>
-  </si>
-  <si>
-    <t>butcher</t>
-  </si>
-  <si>
-    <t>cabinet maker</t>
-  </si>
-  <si>
-    <t>carpenter</t>
-  </si>
-  <si>
-    <t>cashier</t>
-  </si>
-  <si>
-    <t>chaise maker</t>
-  </si>
-  <si>
-    <t>clerk</t>
-  </si>
-  <si>
-    <t>clothier</t>
-  </si>
-  <si>
-    <t>committee</t>
-  </si>
-  <si>
-    <t>comtroller</t>
-  </si>
-  <si>
-    <t>conveyancer</t>
-  </si>
-  <si>
-    <t>cooper</t>
-  </si>
-  <si>
-    <t>cordwainder</t>
-  </si>
-  <si>
-    <t>deacon</t>
-  </si>
-  <si>
-    <t>distiller</t>
-  </si>
-  <si>
-    <t>doctor</t>
-  </si>
-  <si>
-    <t>druggist</t>
-  </si>
-  <si>
-    <t>esq</t>
-  </si>
-  <si>
-    <t>estate</t>
-  </si>
-  <si>
-    <t>excuetor</t>
-  </si>
-  <si>
-    <t>farmer</t>
-  </si>
-  <si>
-    <t>frederick company</t>
-  </si>
-  <si>
-    <t>furrier</t>
-  </si>
-  <si>
-    <t>gentleman</t>
-  </si>
-  <si>
-    <t>glazier</t>
-  </si>
-  <si>
-    <t>goldsmith</t>
-  </si>
-  <si>
-    <t>guardian</t>
-  </si>
-  <si>
-    <t>hatter</t>
-  </si>
-  <si>
-    <t>housewright</t>
-  </si>
-  <si>
-    <t>individual</t>
-  </si>
-  <si>
-    <t>inn keeper</t>
-  </si>
-  <si>
-    <t>judges</t>
-  </si>
-  <si>
-    <t>labourer</t>
-  </si>
-  <si>
-    <t>leather dresser</t>
-  </si>
-  <si>
-    <t>marchant</t>
-  </si>
-  <si>
-    <t>mariner</t>
-  </si>
-  <si>
-    <t>mason</t>
-  </si>
-  <si>
-    <t>miller</t>
-  </si>
-  <si>
-    <t>molster</t>
-  </si>
-  <si>
-    <t>painter</t>
-  </si>
-  <si>
-    <t>planter</t>
-  </si>
-  <si>
-    <t>post master</t>
-  </si>
-  <si>
-    <t>post rider</t>
-  </si>
-  <si>
-    <t>printer</t>
-  </si>
-  <si>
-    <t>property</t>
-  </si>
-  <si>
-    <t>proprietors</t>
-  </si>
-  <si>
-    <t>reverend</t>
-  </si>
-  <si>
-    <t>sadler</t>
-  </si>
-  <si>
-    <t>school committee</t>
-  </si>
-  <si>
-    <t>school master</t>
-  </si>
-  <si>
-    <t>sheriff</t>
-  </si>
-  <si>
-    <t>ship wright</t>
-  </si>
-  <si>
-    <t>shoemaker</t>
-  </si>
-  <si>
-    <t>shopkeeper</t>
-  </si>
-  <si>
-    <t>silversmith</t>
-  </si>
-  <si>
-    <t>soldier</t>
-  </si>
-  <si>
-    <t>spinster</t>
-  </si>
-  <si>
-    <t>tanner</t>
-  </si>
-  <si>
-    <t>taylor</t>
-  </si>
-  <si>
-    <t>trader</t>
-  </si>
-  <si>
-    <t>treasurer</t>
-  </si>
-  <si>
-    <t>trustee</t>
-  </si>
-  <si>
-    <t>weaver</t>
-  </si>
-  <si>
-    <t>widow</t>
-  </si>
-  <si>
-    <t>wife</t>
   </si>
 </sst>
 </file>
@@ -608,13 +611,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,1280 +630,1508 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>8500.810000000001</v>
+        <v>975180.8060949999</v>
       </c>
       <c r="D2">
-        <v>18</v>
+        <v>669</v>
       </c>
       <c r="E2">
-        <v>472.2672222222223</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>34.89827856025039</v>
+      </c>
+      <c r="F2">
+        <v>1457.669366360239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>7.72</v>
+        <v>251444.82</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E3">
-        <v>7.72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>1.669274908711528</v>
+      </c>
+      <c r="F3">
+        <v>7857.650625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>2416.33</v>
+        <v>184573.597932</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>235</v>
       </c>
       <c r="E4">
-        <v>604.0825</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>12.25873761085029</v>
+      </c>
+      <c r="F4">
+        <v>785.4195656680852</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>24827.9</v>
+        <v>79191.01999999999</v>
       </c>
       <c r="D5">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="E5">
-        <v>709.3685714285715</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>4.173187271778821</v>
+      </c>
+      <c r="F5">
+        <v>989.8877499999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>583.96</v>
+        <v>59143.60000000001</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>274</v>
       </c>
       <c r="E6">
-        <v>116.792</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>14.29316640584246</v>
+      </c>
+      <c r="F6">
+        <v>215.8525547445256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>2365.41</v>
+        <v>41367.31</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="E7">
-        <v>1182.705</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>3.129890453834116</v>
+      </c>
+      <c r="F7">
+        <v>689.4551666666666</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8">
-        <v>3436</v>
+        <v>31947.85</v>
       </c>
       <c r="D8">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="E8">
-        <v>381.7777777777778</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>4.173187271778821</v>
+      </c>
+      <c r="F8">
+        <v>399.348125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9">
-        <v>5268.66</v>
+        <v>25249.72</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E9">
-        <v>1756.22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>2.295252999478352</v>
+      </c>
+      <c r="F9">
+        <v>573.8572727272726</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10">
-        <v>783.0700000000001</v>
+        <v>24827.9</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E10">
-        <v>783.0700000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>1.825769431403234</v>
+      </c>
+      <c r="F10">
+        <v>709.3685714285715</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11">
-        <v>37.35</v>
+        <v>18219.3502</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="E11">
-        <v>37.35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>1.721439749608764</v>
+      </c>
+      <c r="F11">
+        <v>552.1015212121213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12">
-        <v>79191.01999999999</v>
+        <v>15703.01</v>
       </c>
       <c r="D12">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="E12">
-        <v>989.8877499999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>3.286384976525822</v>
+      </c>
+      <c r="F12">
+        <v>249.2541269841269</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13">
-        <v>235.7</v>
+        <v>14122.0561</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="E13">
-        <v>235.7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>2.608242044861763</v>
+      </c>
+      <c r="F13">
+        <v>282.441122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14">
-        <v>74.45999999999999</v>
+        <v>13322.03666666667</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E14">
-        <v>74.45999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>1.669274908711528</v>
+      </c>
+      <c r="F14">
+        <v>416.3136458333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15">
-        <v>784.3000000000001</v>
+        <v>8500.810000000001</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E15">
-        <v>78.43000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>0.9389671361502347</v>
+      </c>
+      <c r="F15">
+        <v>472.2672222222223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16">
-        <v>85.3</v>
+        <v>8055.24</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E16">
-        <v>42.65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>0.5216484089723527</v>
+      </c>
+      <c r="F16">
+        <v>805.524</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C17">
-        <v>47.57</v>
+        <v>7083.53</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
-        <v>47.57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F17">
+        <v>7083.53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18">
-        <v>3997</v>
+        <v>5802.73</v>
       </c>
       <c r="D18">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E18">
-        <v>307.4615384615385</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>0.3651538862806468</v>
+      </c>
+      <c r="F18">
+        <v>828.9614285714285</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C19">
-        <v>53.33</v>
+        <v>5268.66</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>53.33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>0.1564945226917058</v>
+      </c>
+      <c r="F19">
+        <v>1756.22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C20">
-        <v>863.41</v>
+        <v>4922.43</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20">
-        <v>287.8033333333333</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>0.1043296817944705</v>
+      </c>
+      <c r="F20">
+        <v>2461.215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C21">
-        <v>53.74</v>
+        <v>3997</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E21">
-        <v>53.74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>0.6781429316640584</v>
+      </c>
+      <c r="F21">
+        <v>307.4615384615385</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C22">
-        <v>108.4</v>
+        <v>3856.94</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E22">
-        <v>108.4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>0.6259780907668232</v>
+      </c>
+      <c r="F22">
+        <v>321.4116666666667</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C23">
-        <v>1720.91</v>
+        <v>3644.93</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E23">
-        <v>430.2275</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>0.4694835680751174</v>
+      </c>
+      <c r="F23">
+        <v>404.9922222222223</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C24">
-        <v>281.25</v>
+        <v>3524.74</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24">
-        <v>281.25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F24">
+        <v>3524.74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C25">
-        <v>16.35</v>
+        <v>3436</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E25">
-        <v>16.35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>0.4694835680751174</v>
+      </c>
+      <c r="F25">
+        <v>381.7777777777778</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C26">
-        <v>466.2500000000001</v>
+        <v>3434.96</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E26">
-        <v>155.4166666666667</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>0.6259780907668232</v>
+      </c>
+      <c r="F26">
+        <v>286.2466666666667</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C27">
-        <v>25249.72</v>
+        <v>3363.41</v>
       </c>
       <c r="D27">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="E27">
-        <v>573.8572727272726</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>0.3129890453834116</v>
+      </c>
+      <c r="F27">
+        <v>560.5683333333333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C28">
-        <v>4922.43</v>
+        <v>3300.5</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E28">
-        <v>2461.215</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>0.7303077725612936</v>
+      </c>
+      <c r="F28">
+        <v>235.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C29">
-        <v>184573.597932</v>
+        <v>3107.18</v>
       </c>
       <c r="D29">
-        <v>235</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>785.4195656680852</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F29">
+        <v>3107.18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C30">
-        <v>1979.6</v>
+        <v>2701.986666666667</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E30">
-        <v>989.8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>0.3129890453834116</v>
+      </c>
+      <c r="F30">
+        <v>450.3311111111111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C31">
-        <v>18219.3502</v>
+        <v>2439.02</v>
       </c>
       <c r="D31">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="E31">
-        <v>552.1015212121213</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F31">
+        <v>2439.02</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C32">
-        <v>59143.60000000001</v>
+        <v>2416.33</v>
       </c>
       <c r="D32">
-        <v>274</v>
+        <v>4</v>
       </c>
       <c r="E32">
-        <v>215.8525547445256</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>0.208659363588941</v>
+      </c>
+      <c r="F32">
+        <v>604.0825</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C33">
-        <v>206.67</v>
+        <v>2365.41</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33">
-        <v>206.67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>0.1043296817944705</v>
+      </c>
+      <c r="F33">
+        <v>1182.705</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C34">
-        <v>3107.18</v>
+        <v>2344.9</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E34">
-        <v>3107.18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>0.1564945226917058</v>
+      </c>
+      <c r="F34">
+        <v>781.6333333333333</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C35">
-        <v>41367.31</v>
+        <v>2282.8</v>
       </c>
       <c r="D35">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="E35">
-        <v>689.4551666666666</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>0.208659363588941</v>
+      </c>
+      <c r="F35">
+        <v>570.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C36">
-        <v>982.35</v>
+        <v>2278.5</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E36">
-        <v>982.35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>0.1564945226917058</v>
+      </c>
+      <c r="F36">
+        <v>759.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C37">
-        <v>1020.36</v>
+        <v>2257.18</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>255.09</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F37">
+        <v>2257.18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C38">
-        <v>5802.73</v>
+        <v>2018.35</v>
       </c>
       <c r="D38">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E38">
-        <v>828.9614285714285</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>0.2608242044861763</v>
+      </c>
+      <c r="F38">
+        <v>403.67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C39">
-        <v>3363.41</v>
+        <v>1979.6</v>
       </c>
       <c r="D39">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E39">
-        <v>560.5683333333333</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>0.1043296817944705</v>
+      </c>
+      <c r="F39">
+        <v>989.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C40">
-        <v>266.67</v>
+        <v>1917.65</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E40">
-        <v>266.67</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>0.1043296817944705</v>
+      </c>
+      <c r="F40">
+        <v>958.8249999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C41">
-        <v>846.23</v>
+        <v>1720.91</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E41">
-        <v>846.23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>0.208659363588941</v>
+      </c>
+      <c r="F41">
+        <v>430.2275</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C42">
-        <v>3300.5</v>
+        <v>1152.5</v>
       </c>
       <c r="D42">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E42">
-        <v>235.75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>0.1564945226917058</v>
+      </c>
+      <c r="F42">
+        <v>384.1666666666667</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C43">
-        <v>2257.18</v>
+        <v>1071.65</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E43">
-        <v>2257.18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>0.3651538862806468</v>
+      </c>
+      <c r="F43">
+        <v>153.0928571428571</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C44">
-        <v>67.16</v>
+        <v>1020.36</v>
       </c>
       <c r="D44">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E44">
-        <v>33.58</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>0.208659363588941</v>
+      </c>
+      <c r="F44">
+        <v>255.09</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C45">
-        <v>666.67</v>
+        <v>982.35</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
       <c r="E45">
-        <v>666.67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F45">
+        <v>982.35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C46">
-        <v>975180.8060949999</v>
+        <v>863.41</v>
       </c>
       <c r="D46">
-        <v>669</v>
+        <v>3</v>
       </c>
       <c r="E46">
-        <v>1457.669366360239</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>0.1564945226917058</v>
+      </c>
+      <c r="F46">
+        <v>287.8033333333333</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C47">
-        <v>14122.0561</v>
+        <v>846.23</v>
       </c>
       <c r="D47">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E47">
-        <v>282.441122</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F47">
+        <v>846.23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C48">
-        <v>1152.5</v>
+        <v>812.9400000000001</v>
       </c>
       <c r="D48">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E48">
-        <v>384.1666666666667</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>0.4173187271778821</v>
+      </c>
+      <c r="F48">
+        <v>101.6175</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C49">
-        <v>18.99</v>
+        <v>784.3000000000001</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E49">
-        <v>18.99</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>0.5216484089723527</v>
+      </c>
+      <c r="F49">
+        <v>78.43000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C50">
-        <v>211.38</v>
+        <v>783.0700000000001</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
       <c r="E50">
-        <v>211.38</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F50">
+        <v>783.0700000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C51">
-        <v>48.61</v>
+        <v>676.91</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E51">
-        <v>48.61</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>0.1564945226917058</v>
+      </c>
+      <c r="F51">
+        <v>225.6366666666667</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C52">
-        <v>13322.03666666667</v>
+        <v>666.67</v>
       </c>
       <c r="D52">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E52">
-        <v>416.3136458333333</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F52">
+        <v>666.67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C53">
-        <v>7083.53</v>
+        <v>583.96</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E53">
-        <v>7083.53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>0.2608242044861763</v>
+      </c>
+      <c r="F53">
+        <v>116.792</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C54">
-        <v>676.91</v>
+        <v>466.2500000000001</v>
       </c>
       <c r="D54">
         <v>3</v>
       </c>
       <c r="E54">
-        <v>225.6366666666667</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+        <v>0.1564945226917058</v>
+      </c>
+      <c r="F54">
+        <v>155.4166666666667</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C55">
-        <v>8055.24</v>
+        <v>461.11</v>
       </c>
       <c r="D55">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E55">
-        <v>805.524</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F55">
+        <v>461.11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C56">
-        <v>461.11</v>
+        <v>335.54</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E56">
-        <v>461.11</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+        <v>0.1043296817944705</v>
+      </c>
+      <c r="F56">
+        <v>167.77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C57">
-        <v>335.54</v>
+        <v>281.25</v>
       </c>
       <c r="D57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E57">
-        <v>167.77</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F57">
+        <v>281.25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C58">
-        <v>2278.5</v>
+        <v>266.67</v>
       </c>
       <c r="D58">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E58">
-        <v>759.5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F58">
+        <v>266.67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C59">
-        <v>3524.74</v>
+        <v>235.7</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59">
-        <v>3524.74</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F59">
+        <v>235.7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C60">
-        <v>1071.65</v>
+        <v>211.38</v>
       </c>
       <c r="D60">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E60">
-        <v>153.0928571428571</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F60">
+        <v>211.38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C61">
-        <v>2344.9</v>
+        <v>206.67</v>
       </c>
       <c r="D61">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E61">
-        <v>781.6333333333333</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F61">
+        <v>206.67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C62">
-        <v>2701.986666666667</v>
+        <v>108.4</v>
       </c>
       <c r="D62">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E62">
-        <v>450.3311111111111</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F62">
+        <v>108.4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C63">
-        <v>2018.35</v>
+        <v>85.3</v>
       </c>
       <c r="D63">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E63">
-        <v>403.67</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+        <v>0.1043296817944705</v>
+      </c>
+      <c r="F63">
+        <v>42.65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C64">
-        <v>3856.94</v>
+        <v>78.48</v>
       </c>
       <c r="D64">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E64">
-        <v>321.4116666666667</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F64">
+        <v>78.48</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C65">
-        <v>812.9400000000001</v>
+        <v>74.45999999999999</v>
       </c>
       <c r="D65">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E65">
-        <v>101.6175</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F65">
+        <v>74.45999999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C66">
-        <v>1917.65</v>
+        <v>67.16</v>
       </c>
       <c r="D66">
         <v>2</v>
       </c>
       <c r="E66">
-        <v>958.8249999999999</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+        <v>0.1043296817944705</v>
+      </c>
+      <c r="F66">
+        <v>33.58</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C67">
-        <v>78.48</v>
+        <v>63.64</v>
       </c>
       <c r="D67">
         <v>1</v>
       </c>
       <c r="E67">
-        <v>78.48</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F67">
+        <v>63.64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C68">
-        <v>3434.96</v>
+        <v>53.74</v>
       </c>
       <c r="D68">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E68">
-        <v>286.2466666666667</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F68">
+        <v>53.74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C69">
-        <v>2282.8</v>
+        <v>53.33</v>
       </c>
       <c r="D69">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E69">
-        <v>570.7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F69">
+        <v>53.33</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C70">
-        <v>3644.93</v>
+        <v>48.61</v>
       </c>
       <c r="D70">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E70">
-        <v>404.9922222222223</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F70">
+        <v>48.61</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C71">
-        <v>15703.01</v>
+        <v>47.57</v>
       </c>
       <c r="D71">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E71">
-        <v>249.2541269841269</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F71">
+        <v>47.57</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C72">
-        <v>251444.82</v>
+        <v>46.02</v>
       </c>
       <c r="D72">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E72">
-        <v>7857.650625</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F72">
+        <v>46.02</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C73">
-        <v>2439.02</v>
+        <v>37.35</v>
       </c>
       <c r="D73">
         <v>1</v>
       </c>
       <c r="E73">
-        <v>2439.02</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F73">
+        <v>37.35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C74">
-        <v>46.02</v>
+        <v>18.99</v>
       </c>
       <c r="D74">
         <v>1</v>
       </c>
       <c r="E74">
-        <v>46.02</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F74">
+        <v>18.99</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C75">
-        <v>31947.85</v>
+        <v>16.35</v>
       </c>
       <c r="D75">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="E75">
-        <v>399.348125</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F75">
+        <v>16.35</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C76">
-        <v>63.64</v>
+        <v>7.72</v>
       </c>
       <c r="D76">
         <v>1</v>
       </c>
       <c r="E76">
-        <v>63.64</v>
+        <v>0.05216484089723526</v>
+      </c>
+      <c r="F76">
+        <v>7.72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>